<commit_message>
[Fix] Excel read error [Fix] Update Excel import template
</commit_message>
<xml_diff>
--- a/public/download/入库信息导入表.xlsx
+++ b/public/download/入库信息导入表.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\501411\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24450" windowHeight="9480"/>
+    <workbookView windowWidth="29620" windowHeight="12789"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -23,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
   <si>
     <r>
       <rPr>
@@ -31,7 +26,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>(</t>
     </r>
@@ -51,7 +46,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>)</t>
     </r>
@@ -81,7 +76,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>2GB
 4GB
@@ -106,7 +101,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>200GB</t>
     </r>
@@ -127,7 +122,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>250G
 320G
@@ -148,193 +143,335 @@
     </r>
   </si>
   <si>
-    <t>资产编号</t>
-  </si>
-  <si>
-    <t>机器名称</t>
-  </si>
-  <si>
-    <t>SN</t>
-  </si>
-  <si>
-    <t>PN</t>
-  </si>
-  <si>
-    <t>部门</t>
-  </si>
-  <si>
-    <t>课</t>
-  </si>
-  <si>
-    <t>状态</t>
-  </si>
-  <si>
-    <t>发票号码</t>
-  </si>
-  <si>
-    <t>流水号码</t>
-  </si>
-  <si>
-    <t>CpuType/CpuValue</t>
-  </si>
-  <si>
-    <t>LCD</t>
-  </si>
-  <si>
-    <t>MEMO</t>
-  </si>
-  <si>
-    <t>HDD</t>
-  </si>
-  <si>
-    <t>CD-ROM</t>
-  </si>
-  <si>
-    <t>位置</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>DT部</t>
-  </si>
-  <si>
-    <t>SWV</t>
-  </si>
-  <si>
-    <t>在库</t>
-  </si>
-  <si>
-    <t>iEXPn(Des)201908-0009</t>
-  </si>
-  <si>
-    <t>24GB</t>
-  </si>
-  <si>
-    <t>1TB</t>
-  </si>
-  <si>
-    <t>ZD102073H</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>DVD-ROM
 DVD-RW
 DVD-BD
 None DVD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>资产编号</t>
+  </si>
+  <si>
+    <t>机器名称</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>部门</t>
+  </si>
+  <si>
+    <t>课</t>
+  </si>
+  <si>
+    <t>状态</t>
+  </si>
+  <si>
+    <t>发票号码</t>
+  </si>
+  <si>
+    <t>流水号码</t>
+  </si>
+  <si>
+    <t>CpuType/CpuValue</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>MEMO</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>CD-ROM</t>
+  </si>
+  <si>
+    <t>位置</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>Altair MZ10 CS2 2U-3 for TECS</t>
+  </si>
+  <si>
+    <t>ZD102073H</t>
+  </si>
+  <si>
+    <t>PMZ12U-AAA27</t>
+  </si>
+  <si>
+    <t>DT部</t>
+  </si>
+  <si>
+    <t>SWV</t>
+  </si>
+  <si>
+    <t>在库</t>
+  </si>
+  <si>
+    <t>iEXPn(Des)201908-0009</t>
+  </si>
+  <si>
+    <t>i7-8650U</t>
+  </si>
+  <si>
+    <t>24GB</t>
+  </si>
+  <si>
+    <t>1TB</t>
   </si>
   <si>
     <t>DVD-ROM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>余瑞馨</t>
   </si>
   <si>
     <t>HWV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>史洪权</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MED</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>余瑞馨</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>i7-8650U</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Altair MZ10 CS2 2U-3 for TECS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CUD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>李雪</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HWD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>刘均凯</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CSV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>王彦</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PSD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>吴樯</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SYD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>居蓉芳</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SCD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>郭宏记</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SSD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>程斌</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>FWD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>林文哲</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMZ12U-AAA27</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -342,7 +479,7 @@
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -351,43 +488,202 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -400,28 +696,270 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -438,11 +976,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,27 +988,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -481,7 +1063,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -519,7 +1101,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,7 +1136,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,38 +1339,40 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="33.375" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="33.3790322580645" customWidth="1"/>
+    <col min="3" max="3" width="13.6290322580645" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="16.75" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="20.75" customWidth="1"/>
-    <col min="9" max="9" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="17.3790322580645" customWidth="1"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="6.625" customWidth="1"/>
+    <col min="11" max="11" width="6.62903225806452" customWidth="1"/>
     <col min="12" max="12" width="7.5" customWidth="1"/>
-    <col min="13" max="13" width="9.625" customWidth="1"/>
-    <col min="14" max="14" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.375" customWidth="1"/>
+    <col min="13" max="13" width="9.62903225806452" customWidth="1"/>
+    <col min="14" max="14" width="9.37903225806452" customWidth="1"/>
+    <col min="15" max="15" width="10.3790322580645" customWidth="1"/>
     <col min="16" max="16" width="20.5" customWidth="1"/>
     <col min="17" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="101.25" x14ac:dyDescent="0.2">
+    <row r="1" ht="97.55" spans="1:16">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -797,7 +1381,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -811,199 +1395,206 @@
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    <row r="2" ht="27.85" spans="1:16">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="N2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="P2" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" s="1" customFormat="1" ht="25.5" customHeight="1" spans="1:16">
       <c r="A3" s="6">
-        <v>1908356</v>
+        <v>1908200</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:P3"/>
-  <dataConsolidate/>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+  <autoFilter ref="A2:P3">
+    <extLst/>
+  </autoFilter>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F65483">
       <formula1>"442,462,485,491,499,520,540,1884,2271,2272,2273,2274"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G65483">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E4:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3">
       <formula1>"DT部,VT部,SWT部"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
       <formula1>"SYD,HWD,MED,CSV,HWV,SSD,SCD,SWV,PSD,CUD,FWD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3">
       <formula1>"在库,待借出审批,待分配,使用中,待报废审批,报废"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A3 A4:A1048576">
       <formula1>COUNTIF(A:A,A1)=1</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E65483">
+      <formula1>"29,33,37"</formula1>
+    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1011,7 +1602,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1019,7 +1610,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1027,7 +1618,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1036,7 +1627,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] actual_price/tax_inclusive_price to excel formatter
</commit_message>
<xml_diff>
--- a/public/download/入库信息导入表.xlsx
+++ b/public/download/入库信息导入表.xlsx
@@ -11,14 +11,14 @@
     <sheet name="links" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">template!$A$2:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">template!$A$2:$R$3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
   <si>
     <r>
       <rPr>
@@ -170,6 +170,12 @@
     <t>状态</t>
   </si>
   <si>
+    <t>实际价格</t>
+  </si>
+  <si>
+    <t>含税价格</t>
+  </si>
+  <si>
     <t>发票号码</t>
   </si>
   <si>
@@ -228,6 +234,9 @@
   </si>
   <si>
     <t>DVD-ROM</t>
+  </si>
+  <si>
+    <t>备注1</t>
   </si>
   <si>
     <t>MED</t>
@@ -294,11 +303,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -339,52 +349,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,6 +417,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -406,17 +456,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,51 +482,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -498,43 +508,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,139 +688,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,156 +828,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -991,8 +1004,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1345,7 +1358,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1360,165 +1373,175 @@
     <col min="5" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="16.75" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="20.75" customWidth="1"/>
-    <col min="9" max="9" width="17.3790322580645" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="6.62903225806452" customWidth="1"/>
-    <col min="12" max="12" width="7.5" customWidth="1"/>
-    <col min="13" max="13" width="9.62903225806452" customWidth="1"/>
-    <col min="14" max="14" width="9.37903225806452" customWidth="1"/>
-    <col min="15" max="15" width="10.3790322580645" customWidth="1"/>
-    <col min="16" max="16" width="20.5" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="2"/>
+    <col min="8" max="9" width="9" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.75" customWidth="1"/>
+    <col min="11" max="11" width="17.3790322580645" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="6.62903225806452" customWidth="1"/>
+    <col min="14" max="14" width="7.5" customWidth="1"/>
+    <col min="15" max="15" width="9.62903225806452" customWidth="1"/>
+    <col min="16" max="16" width="9.37903225806452" customWidth="1"/>
+    <col min="17" max="17" width="10.3790322580645" customWidth="1"/>
+    <col min="18" max="18" width="20.5" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="97.55" spans="1:16">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" ht="97.55" spans="1:18">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="10" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="O1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
-    <row r="2" ht="27.85" spans="1:16">
-      <c r="A2" s="5" t="s">
+    <row r="2" ht="27.85" spans="1:18">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="Q2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="25.5" customHeight="1" spans="1:16">
-      <c r="A3" s="6">
-        <v>1908200</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
+    <row r="3" s="1" customFormat="1" ht="25.5" customHeight="1" spans="1:18">
+      <c r="A3" s="7">
+        <v>1912303</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
+      <c r="H3" s="10">
+        <v>4000.12</v>
+      </c>
+      <c r="I3" s="10">
+        <v>300</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="K3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="M3" s="7">
+        <v>15.6</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="O3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:P3">
+  <autoFilter ref="A2:R3">
     <extLst/>
   </autoFilter>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F65483">
-      <formula1>"442,462,485,491,499,520,540,1884,2271,2272,2273,2274"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G65483">
-      <formula1>"0,1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E4:E1048576">
       <formula1>"DT部,VT部,SWT部"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4:F1048576">
       <formula1>"SYD,HWD,MED,CSV,HWV,SSD,SCD,SWV,PSD,CUD,FWD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G1048576">
       <formula1>"在库,待借出审批,待分配,使用中,待报废审批,报废"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A3 A4:A1048576">
       <formula1>COUNTIF(A:A,A1)=1</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E65483">
-      <formula1>"29,33,37"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1540,90 +1563,90 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Add] category for excel import
</commit_message>
<xml_diff>
--- a/public/download/入库信息导入表.xlsx
+++ b/public/download/入库信息导入表.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29620" windowHeight="12789"/>
+    <workbookView windowWidth="28695" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
     <sheet name="links" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">template!$A$2:$R$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">template!$A$2:$S$3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
   <si>
     <r>
       <rPr>
@@ -155,6 +155,9 @@
     <t>机器名称</t>
   </si>
   <si>
+    <t>区分</t>
+  </si>
+  <si>
     <t>SN</t>
   </si>
   <si>
@@ -204,6 +207,9 @@
   </si>
   <si>
     <t>Altair MZ10 CS2 2U-3 for TECS</t>
+  </si>
+  <si>
+    <t>Altair-MZ0</t>
   </si>
   <si>
     <t>ZD102073H</t>
@@ -305,8 +311,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -342,14 +348,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,26 +369,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -393,17 +392,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,6 +460,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,61 +478,16 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -508,19 +514,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,97 +676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,61 +694,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,33 +732,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -768,17 +747,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,11 +773,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,153 +794,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1076,7 +1082,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="363636"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1358,65 +1364,67 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="33.3790322580645" customWidth="1"/>
-    <col min="3" max="3" width="13.6290322580645" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="16.75" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="9" width="9" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.75" customWidth="1"/>
-    <col min="11" max="11" width="17.3790322580645" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
-    <col min="13" max="13" width="6.62903225806452" customWidth="1"/>
-    <col min="14" max="14" width="7.5" customWidth="1"/>
-    <col min="15" max="15" width="9.62903225806452" customWidth="1"/>
-    <col min="16" max="16" width="9.37903225806452" customWidth="1"/>
-    <col min="17" max="17" width="10.3790322580645" customWidth="1"/>
-    <col min="18" max="18" width="20.5" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="3"/>
+    <col min="2" max="2" width="33.375" customWidth="1"/>
+    <col min="3" max="3" width="21.25" customWidth="1"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="16.75" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="10" width="9" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.75" customWidth="1"/>
+    <col min="12" max="12" width="17.375" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="6.625" customWidth="1"/>
+    <col min="15" max="15" width="7.5" customWidth="1"/>
+    <col min="16" max="16" width="9.625" customWidth="1"/>
+    <col min="17" max="17" width="9.375" customWidth="1"/>
+    <col min="18" max="18" width="10.375" customWidth="1"/>
+    <col min="19" max="19" width="20.5" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="97.55" spans="1:18">
+    <row r="1" ht="94.5" spans="1:19">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="5"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="9"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="4"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
     </row>
-    <row r="2" ht="27.85" spans="1:18">
+    <row r="2" ht="27" spans="1:19">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1471,73 +1479,79 @@
       <c r="R2" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="S2" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="25.5" customHeight="1" spans="1:18">
+    <row r="3" s="1" customFormat="1" ht="25.5" customHeight="1" spans="1:19">
       <c r="A3" s="7">
-        <v>1912303</v>
+        <v>3912303</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="C3" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="E3" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="F3" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="10">
+        <v>29</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="10">
         <v>4000.12</v>
       </c>
-      <c r="I3" s="10">
+      <c r="J3" s="10">
         <v>300</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="K3" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="7">
+        <v>31</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="7">
         <v>15.6</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="O3" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R3">
+  <autoFilter ref="A2:S3">
     <extLst/>
   </autoFilter>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E4:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4:F1048576">
       <formula1>"DT部,VT部,SWT部"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G1048576">
       <formula1>"SYD,HWD,MED,CSV,HWV,SSD,SCD,SWV,PSD,CUD,FWD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H4:H1048576">
       <formula1>"在库,待借出审批,待分配,使用中,待报废审批,报废"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A3 A4:A1048576">
@@ -1559,94 +1573,94 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Update] ems_admin has scrap right [Add] NPI/FATN
</commit_message>
<xml_diff>
--- a/public/download/入库信息导入表.xlsx
+++ b/public/download/入库信息导入表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="11505"/>
+    <workbookView windowWidth="29620" windowHeight="12789"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <r>
       <rPr>
@@ -304,6 +304,12 @@
   <si>
     <t>林文哲</t>
   </si>
+  <si>
+    <t>FATN</t>
+  </si>
+  <si>
+    <t>葛章峰</t>
+  </si>
 </sst>
 </file>
 
@@ -312,8 +318,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -348,6 +354,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -369,18 +406,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -393,6 +439,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -401,23 +454,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,66 +494,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,19 +520,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +622,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,37 +652,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,13 +670,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,79 +682,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,6 +738,33 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -747,11 +780,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -767,15 +806,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -805,177 +835,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1082,7 +1088,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="363636"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1370,30 +1376,30 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="33.375" customWidth="1"/>
+    <col min="2" max="2" width="33.3790322580645" customWidth="1"/>
     <col min="3" max="3" width="21.25" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="4" max="4" width="13.6290322580645" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="16.75" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="9" max="10" width="9" style="2" customWidth="1"/>
     <col min="11" max="11" width="20.75" customWidth="1"/>
-    <col min="12" max="12" width="17.375" customWidth="1"/>
+    <col min="12" max="12" width="17.3790322580645" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="6.625" customWidth="1"/>
+    <col min="14" max="14" width="6.62903225806452" customWidth="1"/>
     <col min="15" max="15" width="7.5" customWidth="1"/>
-    <col min="16" max="16" width="9.625" customWidth="1"/>
-    <col min="17" max="17" width="9.375" customWidth="1"/>
-    <col min="18" max="18" width="10.375" customWidth="1"/>
+    <col min="16" max="16" width="9.62903225806452" customWidth="1"/>
+    <col min="17" max="17" width="9.37903225806452" customWidth="1"/>
+    <col min="18" max="18" width="10.3790322580645" customWidth="1"/>
     <col min="19" max="19" width="20.5" customWidth="1"/>
     <col min="20" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="94.5" spans="1:19">
+    <row r="1" ht="97.55" spans="1:19">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1424,7 +1430,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" ht="27" spans="1:19">
+    <row r="2" ht="27.85" spans="1:19">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1545,17 +1551,17 @@
     <extLst/>
   </autoFilter>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4:F1048576">
-      <formula1>"DT部,VT部,SWT部"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4:G1048576">
-      <formula1>"SYD,HWD,MED,CSV,HWV,SSD,SCD,SWV,PSD,CUD,FWD"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H4:H1048576">
       <formula1>"在库,待借出审批,待分配,使用中,待报废审批,报废"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A3 A4:A1048576">
       <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
+      <formula1>"DT部,VT部,SWT部,NPI部"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576">
+      <formula1>"SYD,HWD,MED,CSV,HWV,SSD,SCD,SWV,PSD,CUD,FWD,FATN"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1567,13 +1573,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.45" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1661,6 +1667,14 @@
       </c>
       <c r="B11" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>